<commit_message>
Clean up GA-DSI folders - delete Other_DSI and Outcomes
</commit_message>
<xml_diff>
--- a/DSI-copy/projects/projects-weekly/project-05/code/starter-code/model_comp.xlsx
+++ b/DSI-copy/projects/projects-weekly/project-05/code/starter-code/model_comp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="models.no_fare_parch" sheetId="1" r:id="rId1"/>
@@ -423,14 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -440,7 +441,7 @@
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -466,7 +467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -491,8 +492,12 @@
       <c r="H2" s="4">
         <v>0.82779056983599997</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="4">
+        <f>1-F2</f>
+        <v>0.86428571428599998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -517,8 +522,12 @@
       <c r="H3" s="4">
         <v>0.82779587299500001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I8" si="0">1-F3</f>
+        <v>0.87142857142899999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -543,8 +552,12 @@
       <c r="H4" s="4">
         <v>0.82720597369799997</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.86428571428599998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -569,8 +582,12 @@
       <c r="H5" s="4">
         <v>0.82667777437099998</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.86428571428599998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -595,8 +612,12 @@
       <c r="H6" s="4">
         <v>0.83277727248300004</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.87857142857100001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -621,8 +642,12 @@
       <c r="H7" s="4">
         <v>0.76714533179699995</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.94285714285709998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -647,8 +672,12 @@
       <c r="H8" s="4">
         <v>0.813888994644</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.88571428571400002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -674,7 +703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f>A2</f>
         <v>0</v>
@@ -702,13 +731,13 @@
         <v>0.83958924543699998</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <f t="shared" ref="A12:B17" si="0">A3</f>
+        <f t="shared" ref="A12:B17" si="1">A3</f>
         <v>1</v>
       </c>
       <c r="B12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Logistic Regression CV</v>
       </c>
       <c r="C12" s="4">
@@ -730,13 +759,13 @@
         <v>0.83598144591000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>GridSearch Logistic Regression</v>
       </c>
       <c r="C13" s="4">
@@ -758,13 +787,13 @@
         <v>0.83597599254999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>kNN Model</v>
       </c>
       <c r="C14" s="4">
@@ -786,13 +815,13 @@
         <v>0.81319086293499998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>GridSearch kNN Model</v>
       </c>
       <c r="C15" s="4">
@@ -814,13 +843,13 @@
         <v>0.81319086293499998</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>GridSearch SVM Model</v>
       </c>
       <c r="C16" s="4">
@@ -844,11 +873,11 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>GridSearch Decision Tree Model</v>
       </c>
       <c r="C17" s="4">
@@ -910,33 +939,33 @@
         <v>1.2765957445999954E-2</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" ref="D20:H20" si="1">D11-D2</f>
+        <f t="shared" ref="D20:H20" si="2">D11-D2</f>
         <v>3.4372604139999985E-2</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.0526315788999985E-2</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.8571428570999993E-2</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9699248119999799E-3</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1798675601000008E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <f t="shared" ref="A21:B21" si="2">A12</f>
+        <f t="shared" ref="A21:B21" si="3">A12</f>
         <v>1</v>
       </c>
       <c r="B21" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Logistic Regression CV</v>
       </c>
       <c r="C21" s="4">
@@ -944,33 +973,33 @@
         <v>8.5106382969999395E-3</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" ref="D21:H21" si="3">D12-D3</f>
+        <f t="shared" ref="D21:H21" si="4">D12-D3</f>
         <v>1.8181818181999931E-2</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1.4285714285000015E-2</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6691729330000635E-3</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.1855729149999945E-3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <f t="shared" ref="A22:B22" si="4">A13</f>
+        <f t="shared" ref="A22:B22" si="5">A13</f>
         <v>2</v>
       </c>
       <c r="B22" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>GridSearch Logistic Regression</v>
       </c>
       <c r="C22" s="4">
@@ -978,33 +1007,33 @@
         <v>1.2765957445999954E-2</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" ref="D22:H22" si="5">D13-D4</f>
+        <f t="shared" ref="D22:H22" si="6">D13-D4</f>
         <v>3.4372604139999985E-2</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.0526315788999985E-2</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.8571428570999993E-2</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.79699248200005E-3</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.7700188520000166E-3</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <f t="shared" ref="A23:B23" si="6">A14</f>
+        <f t="shared" ref="A23:B23" si="7">A14</f>
         <v>3</v>
       </c>
       <c r="B23" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>kNN Model</v>
       </c>
       <c r="C23" s="4">
@@ -1012,33 +1041,33 @@
         <v>4.2553191490000142E-3</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" ref="D23:H23" si="7">D14-D5</f>
+        <f t="shared" ref="D23:H23" si="8">D14-D5</f>
         <v>8.9376915220000797E-3</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-7.1428571429999754E-3</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.4135338346000013E-2</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-1.3486911436000004E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <f t="shared" ref="A24:B24" si="8">A15</f>
+        <f t="shared" ref="A24:B24" si="9">A15</f>
         <v>4</v>
       </c>
       <c r="B24" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>GridSearch kNN Model</v>
       </c>
       <c r="C24" s="4">
@@ -1046,33 +1075,33 @@
         <v>1.2765957447000043E-2</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" ref="D24:H24" si="9">D15-D6</f>
+        <f t="shared" ref="D24:H24" si="10">D15-D6</f>
         <v>2.7382256300001462E-4</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.2105263158000006E-2</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.1428571420000114E-3</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.1428571427999921E-2</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.9586409548000061E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <f t="shared" ref="A25:B25" si="10">A16</f>
+        <f t="shared" ref="A25:B25" si="11">A16</f>
         <v>5</v>
       </c>
       <c r="B25" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>GridSearch SVM Model</v>
       </c>
       <c r="C25" s="4">
@@ -1080,33 +1109,33 @@
         <v>-2.127659574499996E-2</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" ref="D25:H25" si="11">D16-D7</f>
+        <f t="shared" ref="D25:H25" si="12">D16-D7</f>
         <v>-5.973364668999992E-2</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.5714285714200003E-2</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.9473684209999989E-2</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.8464901666000064E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <f t="shared" ref="A26:B26" si="12">A17</f>
+        <f t="shared" ref="A26:B26" si="13">A17</f>
         <v>6</v>
       </c>
       <c r="B26" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>GridSearch Decision Tree Model</v>
       </c>
       <c r="C26" s="4">
@@ -1114,23 +1143,23 @@
         <v>4.2553191490000142E-3</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" ref="D26:H26" si="13">D17-D8</f>
+        <f t="shared" ref="D26:H26" si="14">D17-D8</f>
         <v>2.6855969894000076E-2</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-2.1052631579000058E-2</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-2.1428571428899992E-2</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.1766917292999945E-2</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.1721238819000019E-2</v>
       </c>
     </row>

</xml_diff>